<commit_message>
Update example dashboard and data
</commit_message>
<xml_diff>
--- a/example/sample_structures.xlsx
+++ b/example/sample_structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\3dmol.pbiviz\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12B2BF5-6995-46C7-9F43-FF340257B083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79AC902-FD5E-4492-BDC4-582CDE37FCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{39FA5FB8-A442-4F7D-8F77-B12F9AFDB4EE}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{39FA5FB8-A442-4F7D-8F77-B12F9AFDB4EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>5jxe</t>
   </si>
@@ -45,15 +45,6 @@
   </si>
   <si>
     <t>5zmz</t>
-  </si>
-  <si>
-    <t>structure_string</t>
-  </si>
-  <si>
-    <t>structure_type</t>
-  </si>
-  <si>
-    <t>pdb</t>
   </si>
   <si>
     <t xml:space="preserve">ATOM      1  N   MET A   1       0.000   0.000   0.000  1.00  0.00           N  
@@ -86,9 +77,6 @@
   </si>
   <si>
     <t>sample_2</t>
-  </si>
-  <si>
-    <t>sdf</t>
   </si>
   <si>
     <t>`@&lt;TRIPOS&gt;MOLECULE
@@ -145,16 +133,7 @@
     <t>1906_mol2</t>
   </si>
   <si>
-    <t>mol2</t>
-  </si>
-  <si>
-    <t>structure_path</t>
-  </si>
-  <si>
     <t>https://files.rcsb.org/view/5ZMZ.cif</t>
-  </si>
-  <si>
-    <t>cif</t>
   </si>
   <si>
     <t>ATOM   4345  N   ALA G   7     136.474 136.005  65.236  1.00 92.27           N  
@@ -662,6 +641,9 @@
   <si>
     <t>PD-1 with Pembrolizumab (CIF url)</t>
   </si>
+  <si>
+    <t>structure_data</t>
+  </si>
 </sst>
 </file>
 
@@ -1049,171 +1031,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2C5880-0163-413C-81AB-E21D9D0875D5}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="64.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{21E2F597-508E-471A-8AA4-0942FE165034}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{21E2F597-508E-471A-8AA4-0942FE165034}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>